<commit_message>
agregando plan de configuracion
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\escuela1\qualtcom\Organizacional\Configuracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\proyecto\qualtcom\Organizacional\Configuracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -420,13 +420,13 @@
     <t>Calendario_preventivo</t>
   </si>
   <si>
-    <t>Respaldos Se realizan cada semana en dias viernes, Dichos respaldos generan un comprimido semanal con los archivos agregados hasta la fecha y se versionan en el repositorio de GITHUB con el comentario 'respaldo de sistema' cuyo responsible de generar dicha actividad sera : Jovanny Zepeda</t>
-  </si>
-  <si>
     <t>Mantis</t>
   </si>
   <si>
     <t>192.168.220.112/xampp/mantis(Red local qualtop)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respaldos Se realizan cada semana en dias viernes, Dichos respaldos generan un comprimido semanal con los archivos agregados hasta la fecha y se versionan en el repositorio de GITHUB con el comentario 'respaldo de sistema' cuyo responsible de generar dicha actividad sera : Jovanny Zepeda </t>
   </si>
 </sst>
 </file>
@@ -827,6 +827,42 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -836,44 +872,8 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1250,7 +1250,7 @@
   <dimension ref="A1:AMK116"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A59" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+      <selection activeCell="B63" sqref="B63:C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1303,11 +1303,11 @@
   <sheetData>
     <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="24"/>
@@ -1316,19 +1316,19 @@
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
     </row>
     <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
     </row>
     <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -1370,11 +1370,11 @@
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
     </row>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
@@ -1428,11 +1428,11 @@
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -1476,11 +1476,11 @@
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -1504,11 +1504,11 @@
     </row>
     <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
     </row>
     <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="35" t="s">
@@ -1538,11 +1538,11 @@
       <c r="D26" s="37"/>
     </row>
     <row r="27" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
     </row>
     <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="35" t="s">
@@ -1560,11 +1560,11 @@
       <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
     </row>
     <row r="31" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
@@ -1576,11 +1576,11 @@
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="18" t="s">
@@ -1709,11 +1709,11 @@
       <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="22" t="s">
@@ -1727,11 +1727,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="47" t="s">
+      <c r="B50" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
     </row>
     <row r="51" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="23" t="s">
@@ -1755,22 +1755,22 @@
       <c r="D53" s="27"/>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="C54" s="44"/>
+      <c r="C54" s="56"/>
       <c r="D54" s="27"/>
     </row>
     <row r="55" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="50" t="s">
+      <c r="B55" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="C55" s="51"/>
+      <c r="C55" s="50"/>
       <c r="D55" s="27"/>
     </row>
     <row r="56" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="52"/>
-      <c r="C56" s="53"/>
+      <c r="B56" s="51"/>
+      <c r="C56" s="52"/>
       <c r="D56" s="27"/>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1780,22 +1780,22 @@
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
-      <c r="B58" s="46" t="s">
+      <c r="B58" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="46"/>
+      <c r="C58" s="48"/>
       <c r="D58" s="24"/>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="54" t="s">
+      <c r="B59" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="54"/>
+      <c r="C59" s="53"/>
       <c r="D59" s="24"/>
     </row>
     <row r="60" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="54"/>
-      <c r="C60" s="54"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="53"/>
       <c r="D60" s="24"/>
     </row>
     <row r="61" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1805,17 +1805,17 @@
     </row>
     <row r="62" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
-      <c r="B62" s="49" t="s">
+      <c r="B62" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C62" s="49"/>
+      <c r="C62" s="47"/>
       <c r="D62" s="24"/>
     </row>
     <row r="63" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="C63" s="48"/>
+      <c r="B63" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" s="46"/>
       <c r="D63" s="24"/>
     </row>
     <row r="64" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1869,10 +1869,10 @@
     </row>
     <row r="71" spans="1:9" ht="63" x14ac:dyDescent="0.2">
       <c r="B71" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="34" t="s">
         <v>128</v>
-      </c>
-      <c r="C71" s="34" t="s">
-        <v>129</v>
       </c>
       <c r="D71" s="34" t="s">
         <v>57</v>
@@ -2325,17 +2325,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B55:C56"/>
-    <mergeCell ref="B59:C60"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B27:D27"/>
@@ -2343,6 +2332,17 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B55:C56"/>
+    <mergeCell ref="B59:C60"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B15:D15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modificacion sobre el plan de configuracion
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
@@ -394,9 +394,6 @@
     <t>Mecanismos para la generacion de la linea base</t>
   </si>
   <si>
-    <t>Seleccion de los archivos dentro de la terminal git, para agregarlos es necesario ejegutar el comando git add + nombre del archivo linea base , posteriormente se ingresan en una rama secundario del repositorio con el comando git push origin Linea_base</t>
-  </si>
-  <si>
     <r>
       <t>PTL</t>
     </r>
@@ -427,6 +424,9 @@
   </si>
   <si>
     <t>https://github.com/jovannyzepeda/qtp</t>
+  </si>
+  <si>
+    <t>Seleccion de los archivos dentro de la terminal git, para agregarlos es necesario ejegutar el comando git add + nombre del archivo linea base , posteriormente se ingresan en una rama secundario del repositorio con el comando git push origin base</t>
   </si>
 </sst>
 </file>
@@ -836,6 +836,45 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -845,47 +884,8 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1262,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A59" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1316,11 +1316,11 @@
   <sheetData>
     <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="24"/>
@@ -1329,19 +1329,19 @@
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -1383,11 +1383,11 @@
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
     </row>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
@@ -1441,11 +1441,11 @@
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -1489,11 +1489,11 @@
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -1517,11 +1517,11 @@
     </row>
     <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
     </row>
     <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="35" t="s">
@@ -1551,11 +1551,11 @@
       <c r="D26" s="37"/>
     </row>
     <row r="27" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
     </row>
     <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="35" t="s">
@@ -1573,11 +1573,11 @@
       <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
     </row>
     <row r="31" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
@@ -1589,11 +1589,11 @@
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="18" t="s">
@@ -1642,10 +1642,10 @@
     </row>
     <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>125</v>
       </c>
       <c r="D38" s="15"/>
     </row>
@@ -1722,11 +1722,11 @@
       <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="22" t="s">
@@ -1740,11 +1740,11 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="47" t="s">
+      <c r="B50" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
     </row>
     <row r="51" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="23" t="s">
@@ -1768,15 +1768,15 @@
       <c r="D53" s="27"/>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="C54" s="44"/>
+      <c r="C54" s="57"/>
       <c r="D54" s="27"/>
     </row>
     <row r="55" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B55" s="50" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C55" s="51"/>
       <c r="D55" s="27"/>
@@ -1793,15 +1793,15 @@
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
-      <c r="B58" s="46" t="s">
+      <c r="B58" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="46"/>
+      <c r="C58" s="49"/>
       <c r="D58" s="24"/>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B59" s="54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C59" s="54"/>
       <c r="D59" s="24"/>
@@ -1818,17 +1818,17 @@
     </row>
     <row r="62" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
-      <c r="B62" s="49" t="s">
+      <c r="B62" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C62" s="49"/>
+      <c r="C62" s="48"/>
       <c r="D62" s="24"/>
     </row>
     <row r="63" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="C63" s="48"/>
+      <c r="B63" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="47"/>
       <c r="D63" s="24"/>
     </row>
     <row r="64" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1873,8 +1873,8 @@
       <c r="B70" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C70" s="58" t="s">
-        <v>129</v>
+      <c r="C70" s="42" t="s">
+        <v>128</v>
       </c>
       <c r="D70" s="34" t="s">
         <v>55</v>
@@ -1882,10 +1882,10 @@
     </row>
     <row r="71" spans="1:9" ht="63" x14ac:dyDescent="0.2">
       <c r="B71" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C71" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D71" s="34" t="s">
         <v>56</v>
@@ -2338,17 +2338,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B55:C56"/>
-    <mergeCell ref="B59:C60"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B27:D27"/>
@@ -2356,6 +2345,17 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B55:C56"/>
+    <mergeCell ref="B59:C60"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B15:D15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C70" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizando plan de configuracion
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="139">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -442,6 +442,18 @@
   </si>
   <si>
     <t>Registrados en herramienta mantis(Sin direccion fisica en archivos)</t>
+  </si>
+  <si>
+    <t>Minutas de cambios</t>
+  </si>
+  <si>
+    <t>Minuta_cambio-aammdd</t>
+  </si>
+  <si>
+    <t>Bitacora de respaldos</t>
+  </si>
+  <si>
+    <t>Bitacora de respaldos Base de datos</t>
   </si>
 </sst>
 </file>
@@ -666,7 +678,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -779,21 +791,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -901,6 +904,54 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -910,42 +961,6 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -955,26 +970,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1349,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK119"/>
+  <dimension ref="A1:AMK122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1405,19 +1405,19 @@
   <sheetData>
     <row r="1" spans="1:1025" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:1025" s="43" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42"/>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
       <c r="E2" s="26"/>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
@@ -2442,11 +2442,11 @@
     </row>
     <row r="3" spans="1:1025" s="43" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="44"/>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -3471,11 +3471,11 @@
     </row>
     <row r="4" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
     </row>
     <row r="5" spans="1:1025" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -3517,11 +3517,11 @@
     </row>
     <row r="9" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
@@ -3575,11 +3575,11 @@
     </row>
     <row r="15" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -3623,11 +3623,11 @@
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -3651,11 +3651,11 @@
     </row>
     <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
     </row>
     <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="34" t="s">
@@ -3685,11 +3685,11 @@
       <c r="D26" s="36"/>
     </row>
     <row r="27" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
     </row>
     <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="34" t="s">
@@ -3707,11 +3707,11 @@
       <c r="D29" s="24"/>
     </row>
     <row r="30" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
     </row>
     <row r="31" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
@@ -3723,11 +3723,11 @@
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="18" t="s">
@@ -3799,287 +3799,282 @@
       </c>
       <c r="D40" s="17"/>
     </row>
-    <row r="41" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="19" t="s">
+    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="17"/>
+    </row>
+    <row r="42" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-    </row>
-    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A42" s="3"/>
-      <c r="B42" s="18" t="s">
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+    </row>
+    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A43" s="3"/>
+      <c r="B43" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C43" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="D42" s="20"/>
-    </row>
-    <row r="43" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="19" t="s">
+      <c r="D43" s="20"/>
+    </row>
+    <row r="44" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-    </row>
-    <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A44" s="3"/>
-      <c r="B44" s="18" t="s">
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+    </row>
+    <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A45" s="3"/>
+      <c r="B45" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C45" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="20"/>
-    </row>
-    <row r="45" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="19" t="s">
+      <c r="D45" s="20"/>
+    </row>
+    <row r="46" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-    </row>
-    <row r="46" spans="1:4" ht="42" x14ac:dyDescent="0.35">
-      <c r="A46" s="3"/>
-      <c r="B46" s="18" t="s">
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+    </row>
+    <row r="47" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+      <c r="A47" s="3"/>
+      <c r="B47" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C47" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D46" s="20"/>
-    </row>
-    <row r="47" spans="1:4" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="58" t="s">
+      <c r="D47" s="20"/>
+    </row>
+    <row r="48" spans="1:4" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-    </row>
-    <row r="48" spans="1:4" s="4" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="68" t="s">
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+    </row>
+    <row r="49" spans="1:4" s="4" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="C48" s="69" t="s">
+      <c r="C49" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="D48" s="67"/>
-    </row>
-    <row r="49" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="66"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="66"/>
+      <c r="D49" s="46"/>
     </row>
     <row r="50" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="66"/>
-      <c r="C50" s="66"/>
-      <c r="D50" s="66"/>
-    </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="63" t="s">
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+    </row>
+    <row r="51" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="64"/>
-      <c r="D51" s="65"/>
-    </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="21" t="s">
+      <c r="C51" s="65"/>
+      <c r="D51" s="66"/>
+    </row>
+    <row r="52" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" s="68" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="68"/>
+    </row>
+    <row r="53" spans="1:4" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="67"/>
+      <c r="C53" s="67"/>
+      <c r="D53" s="67"/>
+    </row>
+    <row r="54" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
+    </row>
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C52" s="21" t="s">
+      <c r="C55" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D52" s="21" t="s">
+      <c r="D55" s="21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="60" t="s">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C53" s="61"/>
-      <c r="D53" s="62"/>
-    </row>
-    <row r="54" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="22" t="s">
+      <c r="C56" s="65"/>
+      <c r="D56" s="66"/>
+    </row>
+    <row r="57" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C57" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D54" s="22" t="s">
+      <c r="D57" s="22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="26"/>
-    </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="26"/>
-    </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="46" t="s">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="26"/>
+    </row>
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="26"/>
+    </row>
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="47"/>
-      <c r="D57" s="26"/>
-    </row>
-    <row r="58" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="52" t="s">
+      <c r="C60" s="63"/>
+      <c r="D60" s="26"/>
+    </row>
+    <row r="61" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="C58" s="53"/>
-      <c r="D58" s="26"/>
-    </row>
-    <row r="59" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="54"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="26"/>
-    </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="26"/>
-    </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="5"/>
-      <c r="B61" s="49" t="s">
+      <c r="C61" s="57"/>
+      <c r="D61" s="26"/>
+    </row>
+    <row r="62" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="58"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="26"/>
+    </row>
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="26"/>
+    </row>
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="5"/>
+      <c r="B64" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="49"/>
-      <c r="D61" s="23"/>
-    </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="56" t="s">
+      <c r="C64" s="50"/>
+      <c r="D64" s="23"/>
+    </row>
+    <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="C62" s="56"/>
-      <c r="D62" s="23"/>
-    </row>
-    <row r="63" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="56"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="23"/>
-    </row>
-    <row r="64" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B64" s="27"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="23"/>
-    </row>
-    <row r="65" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A65" s="5"/>
-      <c r="B65" s="51" t="s">
+      <c r="C65" s="60"/>
+      <c r="D65" s="23"/>
+    </row>
+    <row r="66" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="60"/>
+      <c r="C66" s="60"/>
+      <c r="D66" s="23"/>
+    </row>
+    <row r="67" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B67" s="27"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="23"/>
+    </row>
+    <row r="68" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A68" s="5"/>
+      <c r="B68" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="51"/>
-      <c r="D65" s="23"/>
-    </row>
-    <row r="66" spans="1:9" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="50" t="s">
+      <c r="C68" s="55"/>
+      <c r="D68" s="23"/>
+    </row>
+    <row r="69" spans="1:9" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="C66" s="50"/>
-      <c r="D66" s="23"/>
-    </row>
-    <row r="67" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B67" s="29"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="23"/>
-    </row>
-    <row r="68" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B68" s="29"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="23"/>
-    </row>
-    <row r="69" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A69" s="6"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
+      <c r="C69" s="54"/>
+      <c r="D69" s="23"/>
     </row>
     <row r="70" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B70" s="31"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="23"/>
     </row>
     <row r="71" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-    </row>
-    <row r="72" spans="1:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="A72" s="5"/>
-      <c r="B72" s="32" t="s">
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="23"/>
+    </row>
+    <row r="72" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A72" s="6"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+    </row>
+    <row r="73" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B73" s="31"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+    </row>
+    <row r="74" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+    </row>
+    <row r="75" spans="1:9" ht="21" x14ac:dyDescent="0.3">
+      <c r="A75" s="5"/>
+      <c r="B75" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C72" s="32" t="s">
+      <c r="C75" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="D72" s="32" t="s">
+      <c r="D75" s="32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="84" x14ac:dyDescent="0.2">
-      <c r="B73" s="33" t="s">
+    <row r="76" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="B76" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C73" s="41" t="s">
+      <c r="C76" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="D73" s="33" t="s">
+      <c r="D76" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="63" x14ac:dyDescent="0.2">
-      <c r="B74" s="33" t="s">
+    <row r="77" spans="1:9" ht="63" x14ac:dyDescent="0.2">
+      <c r="B77" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="C74" s="33" t="s">
+      <c r="C77" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="D74" s="33" t="s">
+      <c r="D77" s="33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B77" s="6"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
-    </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B78" s="6"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6"/>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B79" s="6"/>
@@ -4491,8 +4486,52 @@
       <c r="H119" s="6"/>
       <c r="I119" s="6"/>
     </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
+      <c r="I121" s="6"/>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B122" s="6"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B61:C62"/>
+    <mergeCell ref="B65:C66"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B1:D1"/>
@@ -4500,22 +4539,9 @@
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B58:C59"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B47:D47"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C73" r:id="rId1"/>
+    <hyperlink ref="C76" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Actualizacion plan de configuracion por nombre incorrecto a ruta de bitacora
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="140">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t>Bitacora de respaldos Base de datos</t>
+  </si>
+  <si>
+    <t>Respaldo</t>
   </si>
 </sst>
 </file>
@@ -796,7 +799,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -916,64 +919,73 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1351,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1405,19 +1417,19 @@
   <sheetData>
     <row r="1" spans="1:1025" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
     </row>
     <row r="2" spans="1:1025" s="43" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42"/>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
       <c r="E2" s="26"/>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
@@ -2442,11 +2454,11 @@
     </row>
     <row r="3" spans="1:1025" s="43" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="44"/>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -3471,11 +3483,11 @@
     </row>
     <row r="4" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
     </row>
     <row r="5" spans="1:1025" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -3517,11 +3529,11 @@
     </row>
     <row r="9" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
     </row>
     <row r="10" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
@@ -3575,11 +3587,11 @@
     </row>
     <row r="15" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
     </row>
     <row r="16" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -3623,11 +3635,11 @@
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -3651,11 +3663,11 @@
     </row>
     <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
     </row>
     <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="34" t="s">
@@ -3685,11 +3697,11 @@
       <c r="D26" s="36"/>
     </row>
     <row r="27" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
     </row>
     <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="34" t="s">
@@ -3707,11 +3719,11 @@
       <c r="D29" s="24"/>
     </row>
     <row r="30" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
     </row>
     <row r="31" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
@@ -3723,11 +3735,11 @@
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="18" t="s">
@@ -3860,11 +3872,11 @@
       <c r="D47" s="20"/>
     </row>
     <row r="48" spans="1:4" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="52" t="s">
+      <c r="B48" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
     </row>
     <row r="49" spans="1:4" s="4" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="47" t="s">
@@ -3881,32 +3893,32 @@
       <c r="D50" s="45"/>
     </row>
     <row r="51" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="64" t="s">
+      <c r="B51" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="70"/>
+      <c r="D51" s="71"/>
+    </row>
+    <row r="52" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="50"/>
+    </row>
+    <row r="53" spans="1:4" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="49"/>
+    </row>
+    <row r="54" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="65"/>
-      <c r="D51" s="66"/>
-    </row>
-    <row r="52" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="68" t="s">
-        <v>138</v>
-      </c>
-      <c r="C52" s="68" t="s">
-        <v>137</v>
-      </c>
-      <c r="D52" s="68"/>
-    </row>
-    <row r="53" spans="1:4" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="67"/>
-      <c r="C53" s="67"/>
-      <c r="D53" s="67"/>
-    </row>
-    <row r="54" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="50"/>
-      <c r="D54" s="50"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55"/>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="21" t="s">
@@ -3920,11 +3932,11 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="64" t="s">
+      <c r="B56" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="65"/>
-      <c r="D56" s="66"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="58"/>
     </row>
     <row r="57" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="22" t="s">
@@ -3948,22 +3960,22 @@
       <c r="D59" s="26"/>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="62" t="s">
+      <c r="B60" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="C60" s="63"/>
+      <c r="C60" s="53"/>
       <c r="D60" s="26"/>
     </row>
     <row r="61" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="56" t="s">
+      <c r="B61" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="C61" s="57"/>
+      <c r="C61" s="63"/>
       <c r="D61" s="26"/>
     </row>
     <row r="62" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="58"/>
-      <c r="C62" s="59"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="65"/>
       <c r="D62" s="26"/>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3973,22 +3985,22 @@
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
-      <c r="B64" s="50" t="s">
+      <c r="B64" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="50"/>
+      <c r="C64" s="55"/>
       <c r="D64" s="23"/>
     </row>
     <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="60" t="s">
+      <c r="B65" s="66" t="s">
         <v>123</v>
       </c>
-      <c r="C65" s="60"/>
+      <c r="C65" s="66"/>
       <c r="D65" s="23"/>
     </row>
     <row r="66" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="60"/>
-      <c r="C66" s="60"/>
+      <c r="B66" s="66"/>
+      <c r="C66" s="66"/>
       <c r="D66" s="23"/>
     </row>
     <row r="67" spans="1:9" ht="21" x14ac:dyDescent="0.35">
@@ -3998,17 +4010,17 @@
     </row>
     <row r="68" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
-      <c r="B68" s="55" t="s">
+      <c r="B68" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="C68" s="55"/>
+      <c r="C68" s="61"/>
       <c r="D68" s="23"/>
     </row>
     <row r="69" spans="1:9" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C69" s="54"/>
+      <c r="C69" s="60"/>
       <c r="D69" s="23"/>
     </row>
     <row r="70" spans="1:9" ht="21" x14ac:dyDescent="0.35">
@@ -4518,6 +4530,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B61:C62"/>
+    <mergeCell ref="B65:C66"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B27:D27"/>
@@ -4527,18 +4551,6 @@
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B61:C62"/>
-    <mergeCell ref="B65:C66"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C76" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificacion del plan de configuracion (Integracion de la direccion de servidor mantis tras riesgo de perdida de servidor)
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
@@ -420,9 +420,6 @@
     <t xml:space="preserve">Respaldos Se realizan cada semana en dias viernes, Dichos respaldos generan un comprimido semanal con los archivos agregados hasta la fecha y se versionan en el repositorio de GITHUB con el comentario 'respaldo de sistema' cuyo responsible de generar dicha actividad sera : Jovanny Zepeda </t>
   </si>
   <si>
-    <t>192.168.220.88/xampp/mantis(Red local qualtop)</t>
-  </si>
-  <si>
     <t>https://github.com/jovannyzepeda/qtp</t>
   </si>
   <si>
@@ -457,6 +454,9 @@
   </si>
   <si>
     <t>Plan estratégico + Estimación + Catalogo de Servicios+ Polizas de clientes</t>
+  </si>
+  <si>
+    <t>via.esy.es/mantis</t>
   </si>
 </sst>
 </file>
@@ -925,68 +925,68 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1363,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1417,19 +1417,19 @@
   <sheetData>
     <row r="1" spans="1:1025" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
     </row>
     <row r="2" spans="1:1025" s="43" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42"/>
-      <c r="B2" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="B2" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
       <c r="E2" s="26"/>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
@@ -2454,11 +2454,11 @@
     </row>
     <row r="3" spans="1:1025" s="43" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="44"/>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -3483,11 +3483,11 @@
     </row>
     <row r="4" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
     </row>
     <row r="5" spans="1:1025" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -3529,11 +3529,11 @@
     </row>
     <row r="9" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
     </row>
     <row r="10" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
@@ -3587,11 +3587,11 @@
     </row>
     <row r="15" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
     </row>
     <row r="16" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -3629,17 +3629,17 @@
         <v>107</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D19" s="35"/>
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -3663,11 +3663,11 @@
     </row>
     <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
     </row>
     <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="34" t="s">
@@ -3697,11 +3697,11 @@
       <c r="D26" s="36"/>
     </row>
     <row r="27" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
     </row>
     <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="34" t="s">
@@ -3719,11 +3719,11 @@
       <c r="D29" s="24"/>
     </row>
     <row r="30" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
     </row>
     <row r="31" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
@@ -3735,11 +3735,11 @@
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="18" t="s">
@@ -3813,10 +3813,10 @@
     </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="D41" s="17"/>
     </row>
@@ -3872,18 +3872,18 @@
       <c r="D47" s="20"/>
     </row>
     <row r="48" spans="1:4" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" s="54"/>
-      <c r="D48" s="54"/>
+      <c r="B48" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
     </row>
     <row r="49" spans="1:4" s="4" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="48" t="s">
         <v>132</v>
-      </c>
-      <c r="C49" s="48" t="s">
-        <v>133</v>
       </c>
       <c r="D49" s="46"/>
     </row>
@@ -3893,18 +3893,18 @@
       <c r="D50" s="45"/>
     </row>
     <row r="51" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="69" t="s">
-        <v>138</v>
-      </c>
-      <c r="C51" s="70"/>
-      <c r="D51" s="71"/>
+      <c r="B51" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="61"/>
+      <c r="D51" s="62"/>
     </row>
     <row r="52" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C52" s="50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D52" s="50"/>
     </row>
@@ -3914,11 +3914,11 @@
       <c r="D53" s="49"/>
     </row>
     <row r="54" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="52" t="s">
+      <c r="B54" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55"/>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="21" t="s">
@@ -3932,11 +3932,11 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="66" t="s">
+      <c r="B56" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="67"/>
-      <c r="D56" s="68"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="58"/>
     </row>
     <row r="57" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="22" t="s">
@@ -3946,7 +3946,7 @@
         <v>48</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3960,22 +3960,22 @@
       <c r="D59" s="26"/>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="64" t="s">
+      <c r="B60" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="C60" s="65"/>
+      <c r="C60" s="53"/>
       <c r="D60" s="26"/>
     </row>
     <row r="61" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="58" t="s">
+      <c r="B61" s="65" t="s">
         <v>121</v>
       </c>
-      <c r="C61" s="59"/>
+      <c r="C61" s="66"/>
       <c r="D61" s="26"/>
     </row>
     <row r="62" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="60"/>
-      <c r="C62" s="61"/>
+      <c r="B62" s="67"/>
+      <c r="C62" s="68"/>
       <c r="D62" s="26"/>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3985,22 +3985,22 @@
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
-      <c r="B64" s="52" t="s">
+      <c r="B64" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="52"/>
+      <c r="C64" s="55"/>
       <c r="D64" s="23"/>
     </row>
     <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="62" t="s">
+      <c r="B65" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="C65" s="62"/>
+      <c r="C65" s="69"/>
       <c r="D65" s="23"/>
     </row>
     <row r="66" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="62"/>
-      <c r="C66" s="62"/>
+      <c r="B66" s="69"/>
+      <c r="C66" s="69"/>
       <c r="D66" s="23"/>
     </row>
     <row r="67" spans="1:9" ht="21" x14ac:dyDescent="0.35">
@@ -4010,17 +4010,17 @@
     </row>
     <row r="68" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
-      <c r="B68" s="57" t="s">
+      <c r="B68" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="57"/>
+      <c r="C68" s="64"/>
       <c r="D68" s="23"/>
     </row>
     <row r="69" spans="1:9" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="56" t="s">
+      <c r="B69" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="56"/>
+      <c r="C69" s="63"/>
       <c r="D69" s="23"/>
     </row>
     <row r="70" spans="1:9" ht="21" x14ac:dyDescent="0.35">
@@ -4066,7 +4066,7 @@
         <v>53</v>
       </c>
       <c r="C76" s="41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D76" s="33" t="s">
         <v>54</v>
@@ -4077,7 +4077,7 @@
         <v>125</v>
       </c>
       <c r="C77" s="33" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="D77" s="33" t="s">
         <v>55</v>
@@ -4530,6 +4530,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B61:C62"/>
+    <mergeCell ref="B65:C66"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B27:D27"/>
@@ -4539,18 +4551,6 @@
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B61:C62"/>
-    <mergeCell ref="B65:C66"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C76" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion de plan de configuracion
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="145">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -457,6 +457,21 @@
   </si>
   <si>
     <t>via.esy.es/mantis</t>
+  </si>
+  <si>
+    <t>Plan estratégico + Estimación + Catalogo de Servicios+ Solicitud de cambios</t>
+  </si>
+  <si>
+    <t>Al generar un cambio</t>
+  </si>
+  <si>
+    <t>cambios</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>Linea cambios</t>
   </si>
 </sst>
 </file>
@@ -595,7 +610,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -678,6 +693,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFCFE7F5"/>
       </patternFill>
     </fill>
   </fills>
@@ -799,7 +820,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -925,6 +946,42 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -934,12 +991,6 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -949,9 +1000,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -961,32 +1009,8 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1361,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK122"/>
+  <dimension ref="A1:AMK127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1417,19 +1441,19 @@
   <sheetData>
     <row r="1" spans="1:1025" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
     </row>
     <row r="2" spans="1:1025" s="43" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
       <c r="E2" s="26"/>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
@@ -2454,11 +2478,11 @@
     </row>
     <row r="3" spans="1:1025" s="43" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="44"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -3483,11 +3507,11 @@
     </row>
     <row r="4" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:1025" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -3529,11 +3553,11 @@
     </row>
     <row r="9" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
     </row>
     <row r="10" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
@@ -3587,11 +3611,11 @@
     </row>
     <row r="15" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
     </row>
     <row r="16" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -3635,11 +3659,11 @@
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -3663,11 +3687,11 @@
     </row>
     <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
     </row>
     <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="34" t="s">
@@ -3697,11 +3721,11 @@
       <c r="D26" s="36"/>
     </row>
     <row r="27" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
     </row>
     <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="34" t="s">
@@ -3719,11 +3743,11 @@
       <c r="D29" s="24"/>
     </row>
     <row r="30" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="59" t="s">
+      <c r="B30" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
     </row>
     <row r="31" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
@@ -3735,11 +3759,11 @@
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="18" t="s">
@@ -3872,13 +3896,13 @@
       <c r="D47" s="20"/>
     </row>
     <row r="48" spans="1:4" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="59" t="s">
+      <c r="B48" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-    </row>
-    <row r="49" spans="1:4" s="4" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+    </row>
+    <row r="49" spans="2:4" s="4" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="47" t="s">
         <v>131</v>
       </c>
@@ -3887,19 +3911,19 @@
       </c>
       <c r="D49" s="46"/>
     </row>
-    <row r="50" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="45"/>
       <c r="C50" s="45"/>
       <c r="D50" s="45"/>
     </row>
-    <row r="51" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="60" t="s">
+    <row r="51" spans="2:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="69" t="s">
         <v>137</v>
       </c>
-      <c r="C51" s="61"/>
-      <c r="D51" s="62"/>
-    </row>
-    <row r="52" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C51" s="70"/>
+      <c r="D51" s="71"/>
+    </row>
+    <row r="52" spans="2:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="50" t="s">
         <v>136</v>
       </c>
@@ -3908,19 +3932,19 @@
       </c>
       <c r="D52" s="50"/>
     </row>
-    <row r="53" spans="1:4" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:4" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="49"/>
       <c r="C53" s="49"/>
       <c r="D53" s="49"/>
     </row>
-    <row r="54" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="55" t="s">
+    <row r="54" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="C54" s="55"/>
-      <c r="D54" s="55"/>
-    </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+    </row>
+    <row r="55" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="21" t="s">
         <v>45</v>
       </c>
@@ -3931,16 +3955,16 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="56" t="s">
+    <row r="56" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="57"/>
-      <c r="D56" s="58"/>
-    </row>
-    <row r="57" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="67"/>
+      <c r="D56" s="68"/>
+    </row>
+    <row r="57" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="22" t="s">
-        <v>25</v>
+        <v>143</v>
       </c>
       <c r="C57" s="22" t="s">
         <v>48</v>
@@ -3949,194 +3973,185 @@
         <v>138</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="26"/>
-    </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="26"/>
-    </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="72"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="72"/>
+    </row>
+    <row r="59" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="72"/>
+      <c r="C59" s="72"/>
+      <c r="D59" s="72"/>
+    </row>
+    <row r="60" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" s="52"/>
+      <c r="D60" s="52"/>
+    </row>
+    <row r="61" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" s="67"/>
+      <c r="D62" s="68"/>
+    </row>
+    <row r="63" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="26"/>
+    </row>
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="C60" s="53"/>
-      <c r="D60" s="26"/>
-    </row>
-    <row r="61" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="65" t="s">
+      <c r="C65" s="65"/>
+      <c r="D65" s="26"/>
+    </row>
+    <row r="66" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="C61" s="66"/>
-      <c r="D61" s="26"/>
-    </row>
-    <row r="62" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="67"/>
-      <c r="C62" s="68"/>
-      <c r="D62" s="26"/>
-    </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="26"/>
-    </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="5"/>
-      <c r="B64" s="55" t="s">
+      <c r="C66" s="59"/>
+      <c r="D66" s="26"/>
+    </row>
+    <row r="67" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="60"/>
+      <c r="C67" s="61"/>
+      <c r="D67" s="26"/>
+    </row>
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B68" s="25"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="26"/>
+    </row>
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="5"/>
+      <c r="B69" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="55"/>
-      <c r="D64" s="23"/>
-    </row>
-    <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="69" t="s">
+      <c r="C69" s="52"/>
+      <c r="D69" s="23"/>
+    </row>
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="C65" s="69"/>
-      <c r="D65" s="23"/>
-    </row>
-    <row r="66" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="69"/>
-      <c r="C66" s="69"/>
-      <c r="D66" s="23"/>
-    </row>
-    <row r="67" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B67" s="27"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="23"/>
-    </row>
-    <row r="68" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A68" s="5"/>
-      <c r="B68" s="64" t="s">
+      <c r="C70" s="62"/>
+      <c r="D70" s="23"/>
+    </row>
+    <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="62"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="23"/>
+    </row>
+    <row r="72" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B72" s="27"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="23"/>
+    </row>
+    <row r="73" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A73" s="5"/>
+      <c r="B73" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="64"/>
-      <c r="D68" s="23"/>
-    </row>
-    <row r="69" spans="1:9" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="63" t="s">
+      <c r="C73" s="57"/>
+      <c r="D73" s="23"/>
+    </row>
+    <row r="74" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="63"/>
-      <c r="D69" s="23"/>
-    </row>
-    <row r="70" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B70" s="29"/>
-      <c r="C70" s="29"/>
-      <c r="D70" s="23"/>
-    </row>
-    <row r="71" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B71" s="29"/>
-      <c r="C71" s="29"/>
-      <c r="D71" s="23"/>
-    </row>
-    <row r="72" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A72" s="6"/>
-      <c r="B72" s="30"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
-    </row>
-    <row r="73" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B73" s="31"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
-    </row>
-    <row r="74" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B74" s="28"/>
-      <c r="C74" s="28"/>
-      <c r="D74" s="28"/>
-    </row>
-    <row r="75" spans="1:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="A75" s="5"/>
-      <c r="B75" s="32" t="s">
+      <c r="C74" s="56"/>
+      <c r="D74" s="23"/>
+    </row>
+    <row r="75" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="23"/>
+    </row>
+    <row r="76" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="23"/>
+    </row>
+    <row r="77" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A77" s="6"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+    </row>
+    <row r="78" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B78" s="31"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+    </row>
+    <row r="79" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B79" s="28"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28"/>
+    </row>
+    <row r="80" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="A80" s="5"/>
+      <c r="B80" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C75" s="32" t="s">
+      <c r="C80" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D75" s="32" t="s">
+      <c r="D80" s="32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="84" x14ac:dyDescent="0.2">
-      <c r="B76" s="33" t="s">
+    <row r="81" spans="2:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="B81" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C76" s="41" t="s">
+      <c r="C81" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="D76" s="33" t="s">
+      <c r="D81" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="63" x14ac:dyDescent="0.2">
-      <c r="B77" s="33" t="s">
+    <row r="82" spans="2:9" ht="63" x14ac:dyDescent="0.2">
+      <c r="B82" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="C77" s="33" t="s">
+      <c r="C82" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="D77" s="33" t="s">
+      <c r="D82" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-      <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B81" s="6"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6"/>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
-      <c r="H82" s="6"/>
-      <c r="I82" s="6"/>
-    </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B83" s="6"/>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
-      <c r="G83" s="6"/>
-      <c r="H83" s="6"/>
-      <c r="I83" s="6"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="6"/>
@@ -4528,8 +4543,74 @@
       <c r="H122" s="6"/>
       <c r="I122" s="6"/>
     </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="6"/>
+      <c r="I124" s="6"/>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="6"/>
+      <c r="I125" s="6"/>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
+    </row>
+    <row r="127" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
+      <c r="I127" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="23">
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B66:C67"/>
+    <mergeCell ref="B70:C71"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B1:D1"/>
@@ -4537,23 +4618,9 @@
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B61:C62"/>
-    <mergeCell ref="B65:C66"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B51:D51"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C76" r:id="rId1"/>
+    <hyperlink ref="C81" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Actualizacion de plan de configuracion --integracion linea para cambios
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="145">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -610,7 +610,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,12 +693,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFCFE7F5"/>
       </patternFill>
     </fill>
   </fills>
@@ -820,7 +814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -946,71 +940,68 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1387,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1441,19 +1432,19 @@
   <sheetData>
     <row r="1" spans="1:1025" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
     </row>
     <row r="2" spans="1:1025" s="43" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
       <c r="E2" s="26"/>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
@@ -2478,11 +2469,11 @@
     </row>
     <row r="3" spans="1:1025" s="43" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="44"/>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -3507,11 +3498,11 @@
     </row>
     <row r="4" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
     </row>
     <row r="5" spans="1:1025" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -3553,11 +3544,11 @@
     </row>
     <row r="9" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
     </row>
     <row r="10" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
@@ -3611,11 +3602,11 @@
     </row>
     <row r="15" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
     </row>
     <row r="16" spans="1:1025" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
@@ -3659,11 +3650,11 @@
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -3687,11 +3678,11 @@
     </row>
     <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
     </row>
     <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="34" t="s">
@@ -3721,11 +3712,11 @@
       <c r="D26" s="36"/>
     </row>
     <row r="27" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
     </row>
     <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="34" t="s">
@@ -3743,11 +3734,11 @@
       <c r="D29" s="24"/>
     </row>
     <row r="30" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
     </row>
     <row r="31" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
@@ -3759,11 +3750,11 @@
       <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="18" t="s">
@@ -3896,11 +3887,11 @@
       <c r="D47" s="20"/>
     </row>
     <row r="48" spans="1:4" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="54" t="s">
+      <c r="B48" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="C48" s="54"/>
-      <c r="D48" s="54"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
     </row>
     <row r="49" spans="2:4" s="4" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="47" t="s">
@@ -3917,11 +3908,11 @@
       <c r="D50" s="45"/>
     </row>
     <row r="51" spans="2:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="69" t="s">
+      <c r="B51" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="C51" s="70"/>
-      <c r="D51" s="71"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="62"/>
     </row>
     <row r="52" spans="2:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="50" t="s">
@@ -3938,11 +3929,11 @@
       <c r="D53" s="49"/>
     </row>
     <row r="54" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="52" t="s">
+      <c r="B54" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55"/>
     </row>
     <row r="55" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="21" t="s">
@@ -3956,11 +3947,11 @@
       </c>
     </row>
     <row r="56" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="66" t="s">
+      <c r="B56" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="67"/>
-      <c r="D56" s="68"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="58"/>
     </row>
     <row r="57" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="22" t="s">
@@ -3974,50 +3965,46 @@
       </c>
     </row>
     <row r="58" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="72"/>
-      <c r="C58" s="72"/>
-      <c r="D58" s="72"/>
+      <c r="B58" s="56" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" s="57"/>
+      <c r="D58" s="58"/>
     </row>
     <row r="59" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="72"/>
-      <c r="C59" s="72"/>
-      <c r="D59" s="72"/>
+      <c r="B59" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="60" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="52" t="s">
-        <v>144</v>
-      </c>
-      <c r="C60" s="52"/>
-      <c r="D60" s="52"/>
-    </row>
-    <row r="61" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D61" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" s="67"/>
-      <c r="D62" s="68"/>
-    </row>
-    <row r="63" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="C63" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="D63" s="22" t="s">
-        <v>140</v>
-      </c>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="26"/>
+    </row>
+    <row r="61" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="53"/>
+      <c r="D61" s="26"/>
+    </row>
+    <row r="62" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62" s="66"/>
+      <c r="D62" s="26"/>
+    </row>
+    <row r="63" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="67"/>
+      <c r="C63" s="68"/>
+      <c r="D63" s="26"/>
     </row>
     <row r="64" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" s="25"/>
@@ -4025,133 +4012,129 @@
       <c r="D64" s="26"/>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="C65" s="65"/>
-      <c r="D65" s="26"/>
+      <c r="B65" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="55"/>
+      <c r="D65" s="23"/>
     </row>
     <row r="66" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="58" t="s">
-        <v>121</v>
-      </c>
-      <c r="C66" s="59"/>
-      <c r="D66" s="26"/>
+      <c r="B66" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="69"/>
+      <c r="D66" s="23"/>
     </row>
     <row r="67" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="60"/>
-      <c r="C67" s="61"/>
-      <c r="D67" s="26"/>
+      <c r="B67" s="69"/>
+      <c r="C67" s="69"/>
+      <c r="D67" s="23"/>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="26"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="23"/>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
-      <c r="B69" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" s="52"/>
+      <c r="B69" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" s="64"/>
       <c r="D69" s="23"/>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="62" t="s">
-        <v>122</v>
-      </c>
-      <c r="C70" s="62"/>
+      <c r="B70" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" s="63"/>
       <c r="D70" s="23"/>
     </row>
     <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="62"/>
-      <c r="C71" s="62"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
       <c r="D71" s="23"/>
     </row>
     <row r="72" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B72" s="27"/>
-      <c r="C72" s="28"/>
+      <c r="B72" s="29"/>
+      <c r="C72" s="29"/>
       <c r="D72" s="23"/>
     </row>
     <row r="73" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A73" s="5"/>
-      <c r="B73" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="C73" s="57"/>
-      <c r="D73" s="23"/>
+      <c r="B73" s="30"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
     </row>
     <row r="74" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="C74" s="56"/>
-      <c r="D74" s="23"/>
+      <c r="B74" s="31"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
     </row>
     <row r="75" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B75" s="29"/>
-      <c r="C75" s="29"/>
-      <c r="D75" s="23"/>
-    </row>
-    <row r="76" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B76" s="29"/>
-      <c r="C76" s="29"/>
-      <c r="D76" s="23"/>
-    </row>
-    <row r="77" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B75" s="28"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+    </row>
+    <row r="76" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="B76" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D76" s="32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="84" x14ac:dyDescent="0.2">
       <c r="A77" s="6"/>
-      <c r="B77" s="30"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
-    </row>
-    <row r="78" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B78" s="31"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="28"/>
-    </row>
-    <row r="79" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B79" s="28"/>
-      <c r="C79" s="28"/>
-      <c r="D79" s="28"/>
-    </row>
-    <row r="80" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="B77" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="D77" s="33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="63" x14ac:dyDescent="0.2">
+      <c r="B78" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D78" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
-      <c r="B80" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C80" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D80" s="32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" ht="84" x14ac:dyDescent="0.2">
-      <c r="B81" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C81" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="D81" s="33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="82" spans="2:9" ht="63" x14ac:dyDescent="0.2">
-      <c r="B82" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="C82" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="D82" s="33" t="s">
-        <v>55</v>
-      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="6"/>
@@ -4554,9 +4537,6 @@
       <c r="I123" s="6"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B124" s="6"/>
-      <c r="C124" s="6"/>
-      <c r="D124" s="6"/>
       <c r="E124" s="6"/>
       <c r="F124" s="6"/>
       <c r="G124" s="6"/>
@@ -4564,9 +4544,6 @@
       <c r="I124" s="6"/>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B125" s="6"/>
-      <c r="C125" s="6"/>
-      <c r="D125" s="6"/>
       <c r="E125" s="6"/>
       <c r="F125" s="6"/>
       <c r="G125" s="6"/>
@@ -4574,9 +4551,6 @@
       <c r="I125" s="6"/>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B126" s="6"/>
-      <c r="C126" s="6"/>
-      <c r="D126" s="6"/>
       <c r="E126" s="6"/>
       <c r="F126" s="6"/>
       <c r="G126" s="6"/>
@@ -4584,9 +4558,6 @@
       <c r="I126" s="6"/>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B127" s="6"/>
-      <c r="C127" s="6"/>
-      <c r="D127" s="6"/>
       <c r="E127" s="6"/>
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
@@ -4594,9 +4565,21 @@
       <c r="I127" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="22">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B62:C63"/>
+    <mergeCell ref="B66:C67"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B61:C61"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B20:D20"/>
@@ -4604,23 +4587,10 @@
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B66:C67"/>
-    <mergeCell ref="B70:C71"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B58:D58"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C81" r:id="rId1"/>
+    <hyperlink ref="C77" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Actualizacion de plan de configuracion , nomenclatura acciones correctivas
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguración.xlsx
@@ -346,9 +346,6 @@
     <t>Acciones Correctivas</t>
   </si>
   <si>
-    <t>Acciones_Correctivas-aammdd</t>
-  </si>
-  <si>
     <t>Cronograma Auditorias</t>
   </si>
   <si>
@@ -456,9 +453,6 @@
     <t>Plan estratégico + Estimación + Catalogo de Servicios+ Polizas de clientes</t>
   </si>
   <si>
-    <t>via.esy.es/mantis</t>
-  </si>
-  <si>
     <t>Plan estratégico + Estimación + Catalogo de Servicios+ Solicitud de cambios</t>
   </si>
   <si>
@@ -472,6 +466,12 @@
   </si>
   <si>
     <t>Linea cambios</t>
+  </si>
+  <si>
+    <t>http://via.esy.es/mantis</t>
+  </si>
+  <si>
+    <t>Acciones_Correctivas</t>
   </si>
 </sst>
 </file>
@@ -1378,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD58"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1441,7 +1441,7 @@
     <row r="2" spans="1:1025" s="43" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42"/>
       <c r="B2" s="71" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="71"/>
       <c r="D2" s="71"/>
@@ -3556,7 +3556,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" s="35"/>
     </row>
@@ -3566,7 +3566,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="35"/>
     </row>
@@ -3576,7 +3576,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="35"/>
     </row>
@@ -3586,7 +3586,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" s="35"/>
     </row>
@@ -3596,7 +3596,7 @@
         <v>105</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="D14" s="35"/>
     </row>
@@ -3641,10 +3641,10 @@
     <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D19" s="35"/>
     </row>
@@ -3770,7 +3770,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D34" s="15"/>
     </row>
@@ -3779,7 +3779,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D35" s="15"/>
     </row>
@@ -3788,7 +3788,7 @@
         <v>37</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D36" s="15"/>
     </row>
@@ -3797,16 +3797,16 @@
         <v>38</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D37" s="15"/>
     </row>
     <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>123</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>124</v>
       </c>
       <c r="D38" s="15"/>
     </row>
@@ -3822,16 +3822,16 @@
         <v>33</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40" s="17"/>
     </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>133</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>134</v>
       </c>
       <c r="D41" s="17"/>
     </row>
@@ -3848,7 +3848,7 @@
         <v>39</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D43" s="20"/>
     </row>
@@ -3865,7 +3865,7 @@
         <v>41</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D45" s="20"/>
     </row>
@@ -3882,23 +3882,23 @@
         <v>43</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D47" s="20"/>
     </row>
     <row r="48" spans="1:4" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" s="59"/>
       <c r="D48" s="59"/>
     </row>
     <row r="49" spans="2:4" s="4" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="48" t="s">
         <v>131</v>
-      </c>
-      <c r="C49" s="48" t="s">
-        <v>132</v>
       </c>
       <c r="D49" s="46"/>
     </row>
@@ -3909,17 +3909,17 @@
     </row>
     <row r="51" spans="2:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" s="60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C51" s="61"/>
       <c r="D51" s="62"/>
     </row>
     <row r="52" spans="2:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C52" s="50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D52" s="50"/>
     </row>
@@ -3955,31 +3955,31 @@
     </row>
     <row r="57" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C57" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C58" s="57"/>
       <c r="D58" s="58"/>
     </row>
     <row r="59" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3989,14 +3989,14 @@
     </row>
     <row r="61" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B61" s="52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C61" s="53"/>
       <c r="D61" s="26"/>
     </row>
     <row r="62" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C62" s="66"/>
       <c r="D62" s="26"/>
@@ -4020,7 +4020,7 @@
     </row>
     <row r="66" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B66" s="69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C66" s="69"/>
       <c r="D66" s="23"/>
@@ -4045,7 +4045,7 @@
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C70" s="63"/>
       <c r="D70" s="23"/>
@@ -4093,7 +4093,7 @@
         <v>53</v>
       </c>
       <c r="C77" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D77" s="33" t="s">
         <v>54</v>
@@ -4101,10 +4101,10 @@
     </row>
     <row r="78" spans="1:4" ht="63" x14ac:dyDescent="0.2">
       <c r="B78" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="C78" s="33" t="s">
-        <v>139</v>
+        <v>124</v>
+      </c>
+      <c r="C78" s="41" t="s">
+        <v>143</v>
       </c>
       <c r="D78" s="33" t="s">
         <v>55</v>
@@ -4591,9 +4591,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C77" r:id="rId1"/>
+    <hyperlink ref="C78" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>